<commit_message>
add colors and print recommendations to fuel table
</commit_message>
<xml_diff>
--- a/misc/PCIII-to-logger tps configuration.xlsx
+++ b/misc/PCIII-to-logger tps configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d1da377b1bb6b6b/motor/rsv mille/tuning/logger/diy-afr-tuning/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCBBFFF9-7CB6-4E29-B98D-32494D28DB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{FCBBFFF9-7CB6-4E29-B98D-32494D28DB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EAAE350-F776-417D-925B-FC2B67CBE746}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{8AEB5C11-0F41-498F-9CA7-CF50EB1B9394}"/>
   </bookViews>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62136524-03BD-4F40-99A5-C744AE0E058F}">
-  <dimension ref="B3:D9"/>
+  <dimension ref="B3:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -444,7 +444,7 @@
         <v>100</v>
       </c>
       <c r="C4">
-        <v>26000</v>
+        <v>24130</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -453,7 +453,7 @@
     <row r="5" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C5">
         <f>C4-C3</f>
-        <v>21050</v>
+        <v>19180</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -465,7 +465,7 @@
       </c>
       <c r="C6" s="1">
         <f>B6/$B$4*$C$5+$C$3</f>
-        <v>5371</v>
+        <v>5333.6</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
@@ -477,25 +477,43 @@
       </c>
       <c r="C7" s="1">
         <f>B7/$B$4*$C$5+$C$3</f>
-        <v>5265.75</v>
+        <v>5237.7</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
         <f>B8/$B$4*$C$5+$C$3</f>
-        <v>6002.5</v>
+        <v>5717.2</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
-        <v>1.8</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <f>B9/$B$4*$C$5+$C$3</f>
-        <v>5328.9</v>
+        <v>5909</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10">
+        <v>1.8</v>
+      </c>
+      <c r="C10" s="1">
+        <f>B10/$B$4*$C$5+$C$3</f>
+        <v>5295.24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11">
+        <v>100.8</v>
+      </c>
+      <c r="C11" s="1">
+        <f>B11/$B$4*$C$5+$C$3</f>
+        <v>24283.439999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>